<commit_message>
Idea de nuevo cruce de datos, partido en 5
</commit_message>
<xml_diff>
--- a/TM Coosalud.xlsx
+++ b/TM Coosalud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelipeVillabona\Desktop\Datos-Colombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B30D1C-874C-4A4D-8F2D-B295C42ACFCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F719A-7B74-421E-9F01-26B69626A555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F52510C5-EB37-4AC6-8A02-C05A3AFA757E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>ID C19</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>TM 3</t>
+  </si>
+  <si>
+    <t>Coosalud</t>
+  </si>
+  <si>
+    <t># Carnet</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -129,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +166,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,11 +205,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -194,6 +229,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +548,7 @@
   <dimension ref="B1:AE33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:Y8"/>
+      <selection activeCell="Y8" sqref="V4:Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +716,11 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
@@ -705,6 +747,18 @@
       </c>
       <c r="F13" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>0</v>
@@ -759,6 +813,9 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O14" s="2">
         <v>1</v>
       </c>
@@ -794,6 +851,7 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
+      <c r="G15" s="1"/>
       <c r="O15" s="2">
         <v>2</v>
       </c>
@@ -829,6 +887,7 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
+      <c r="G16" s="1"/>
       <c r="O16" s="2">
         <v>3</v>
       </c>
@@ -864,6 +923,7 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
+      <c r="G17" s="1"/>
       <c r="O17" s="2">
         <v>4</v>
       </c>
@@ -899,6 +959,7 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
+      <c r="G18" s="1"/>
       <c r="O18" s="2">
         <v>5</v>
       </c>
@@ -936,6 +997,7 @@
       <c r="F19" s="1">
         <v>0</v>
       </c>
+      <c r="G19" s="1"/>
       <c r="O19" s="3" t="s">
         <v>5</v>
       </c>
@@ -975,6 +1037,7 @@
       <c r="F20" s="1">
         <v>0</v>
       </c>
+      <c r="G20" s="1"/>
       <c r="O20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1014,6 +1077,7 @@
       <c r="F21" s="1">
         <v>0</v>
       </c>
+      <c r="G21" s="1"/>
       <c r="O21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1053,6 +1117,7 @@
       <c r="F22" s="1">
         <v>0</v>
       </c>
+      <c r="G22" s="1"/>
       <c r="O22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1092,6 +1157,7 @@
       <c r="F23" s="1">
         <v>0</v>
       </c>
+      <c r="G23" s="1"/>
       <c r="O23" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>